<commit_message>
Update github repository name in report
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">GitHub Repository:</t>
   </si>
   <si>
-    <t xml:space="preserve">CS555Project</t>
+    <t xml:space="preserve">https://github.com/elliot-wasem/CS555Project</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint</t>
@@ -753,7 +753,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -832,7 +832,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -937,11 +937,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="22153623"/>
-        <c:axId val="27306574"/>
+        <c:axId val="32036074"/>
+        <c:axId val="21417420"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22153623"/>
+        <c:axId val="32036074"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,14 +973,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27306574"/>
+        <c:crossAx val="21417420"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27306574"/>
+        <c:axId val="21417420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1022,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22153623"/>
+        <c:crossAx val="32036074"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1049,7 +1049,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1154,11 +1154,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="75485223"/>
-        <c:axId val="65913348"/>
+        <c:axId val="57695863"/>
+        <c:axId val="1814669"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75485223"/>
+        <c:axId val="57695863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,14 +1190,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65913348"/>
+        <c:crossAx val="1814669"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65913348"/>
+        <c:axId val="1814669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75485223"/>
+        <c:crossAx val="57695863"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1277,9 +1277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
+      <xdr:colOff>397080</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1288,7 +1288,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3628440"/>
-        <a:ext cx="4916880" cy="2669760"/>
+        <a:ext cx="4916520" cy="2669400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1307,9 +1307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>947880</xdr:colOff>
+      <xdr:colOff>947520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1319,7 +1319,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512000"/>
-          <a:ext cx="1244520" cy="628920"/>
+          <a:ext cx="1244160" cy="628560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1411,9 +1411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497880</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1423,7 +1423,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5581800" y="1486440"/>
-          <a:ext cx="1238400" cy="536040"/>
+          <a:ext cx="1238040" cy="535680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1496,9 +1496,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>63000</xdr:colOff>
+      <xdr:colOff>62640</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1508,7 +1508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2878920" y="1316520"/>
-          <a:ext cx="1093680" cy="798840"/>
+          <a:ext cx="1093320" cy="798480"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1581,9 +1581,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>506880</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1593,7 +1593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1638720"/>
-          <a:ext cx="408960" cy="425880"/>
+          <a:ext cx="408600" cy="425520"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1685,9 +1685,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1697,7 +1697,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4480920" y="1338120"/>
-          <a:ext cx="1079280" cy="743400"/>
+          <a:ext cx="1078920" cy="743040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1770,9 +1770,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>624960</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1782,7 +1782,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734080" y="5127120"/>
-          <a:ext cx="1213200" cy="629640"/>
+          <a:ext cx="1212840" cy="629280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1860,9 +1860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
+      <xdr:colOff>397080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1871,7 +1871,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1480680"/>
-        <a:ext cx="4809600" cy="2666160"/>
+        <a:ext cx="4809240" cy="2665800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1891,8 +1891,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2652,7 +2652,7 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -3061,13 +3061,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="47.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.32"/>

</xml_diff>

<commit_message>
Update URL in report
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -108,7 +108,7 @@
     <t xml:space="preserve">GitHub Repository:</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/elliot-wasem/CS555Project</t>
+    <t xml:space="preserve">https://github.com/gruberma/CS555Project</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint</t>
@@ -753,7 +753,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="14" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -937,11 +937,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="32036074"/>
-        <c:axId val="21417420"/>
+        <c:axId val="96037251"/>
+        <c:axId val="15345546"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32036074"/>
+        <c:axId val="96037251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,14 +973,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21417420"/>
+        <c:crossAx val="15345546"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21417420"/>
+        <c:axId val="15345546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1022,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32036074"/>
+        <c:crossAx val="96037251"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1154,11 +1154,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="57695863"/>
-        <c:axId val="1814669"/>
+        <c:axId val="20885595"/>
+        <c:axId val="31331293"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57695863"/>
+        <c:axId val="20885595"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,14 +1190,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1814669"/>
+        <c:crossAx val="31331293"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1814669"/>
+        <c:axId val="31331293"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57695863"/>
+        <c:crossAx val="20885595"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1277,9 +1277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>397080</xdr:colOff>
+      <xdr:colOff>396720</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1288,7 +1288,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3628440"/>
-        <a:ext cx="4916520" cy="2669400"/>
+        <a:ext cx="4916160" cy="2669040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1307,9 +1307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>947520</xdr:colOff>
+      <xdr:colOff>947160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1319,7 +1319,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512000"/>
-          <a:ext cx="1244160" cy="628560"/>
+          <a:ext cx="1243800" cy="628200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1411,9 +1411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>497880</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1423,7 +1423,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5581800" y="1486440"/>
-          <a:ext cx="1238040" cy="535680"/>
+          <a:ext cx="1237680" cy="535320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1496,9 +1496,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>62640</xdr:colOff>
+      <xdr:colOff>62280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1508,7 +1508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2878920" y="1316520"/>
-          <a:ext cx="1093320" cy="798480"/>
+          <a:ext cx="1092960" cy="798120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1581,9 +1581,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>506520</xdr:colOff>
+      <xdr:colOff>506160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1593,7 +1593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1638720"/>
-          <a:ext cx="408600" cy="425520"/>
+          <a:ext cx="408240" cy="425160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1685,9 +1685,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>92160</xdr:colOff>
+      <xdr:colOff>91800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1697,7 +1697,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4480920" y="1338120"/>
-          <a:ext cx="1078920" cy="743040"/>
+          <a:ext cx="1078560" cy="742680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1770,9 +1770,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>624600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1782,7 +1782,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734080" y="5127120"/>
-          <a:ext cx="1212840" cy="629280"/>
+          <a:ext cx="1212480" cy="628920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1860,9 +1860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>397080</xdr:colOff>
+      <xdr:colOff>396720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1871,7 +1871,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1480680"/>
-        <a:ext cx="4809240" cy="2665800"/>
+        <a:ext cx="4808880" cy="2665440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1892,7 +1892,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update team report after meeting 2
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="197">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -385,6 +385,36 @@
   </si>
   <si>
     <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep doing:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commit code regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrate code regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procrastination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad / dirty code</t>
   </si>
   <si>
     <t xml:space="preserve">Story Description</t>
@@ -753,7 +783,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="14" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -832,7 +862,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -937,11 +967,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="96037251"/>
-        <c:axId val="15345546"/>
+        <c:axId val="10892030"/>
+        <c:axId val="53781701"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96037251"/>
+        <c:axId val="10892030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,14 +1003,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15345546"/>
+        <c:crossAx val="53781701"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15345546"/>
+        <c:axId val="53781701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1052,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96037251"/>
+        <c:crossAx val="10892030"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1049,7 +1079,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1100,7 +1130,7 @@
                   <c:v>9/24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>10/10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -1127,7 +1157,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -1154,11 +1184,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="20885595"/>
-        <c:axId val="31331293"/>
+        <c:axId val="39127851"/>
+        <c:axId val="67559729"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20885595"/>
+        <c:axId val="39127851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,14 +1220,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31331293"/>
+        <c:crossAx val="67559729"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31331293"/>
+        <c:axId val="67559729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1269,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20885595"/>
+        <c:crossAx val="39127851"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1277,9 +1307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>396720</xdr:colOff>
+      <xdr:colOff>396360</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1288,7 +1318,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3628440"/>
-        <a:ext cx="4916160" cy="2669040"/>
+        <a:ext cx="4915800" cy="2668680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1307,9 +1337,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>947160</xdr:colOff>
+      <xdr:colOff>946800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1319,7 +1349,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512000"/>
-          <a:ext cx="1243800" cy="628200"/>
+          <a:ext cx="1243440" cy="627840"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1411,9 +1441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
+      <xdr:colOff>497160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1423,7 +1453,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5581800" y="1486440"/>
-          <a:ext cx="1237680" cy="535320"/>
+          <a:ext cx="1237320" cy="534960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1496,9 +1526,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>62280</xdr:colOff>
+      <xdr:colOff>61920</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1508,7 +1538,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2878920" y="1316520"/>
-          <a:ext cx="1092960" cy="798120"/>
+          <a:ext cx="1092600" cy="797760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1581,9 +1611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>506160</xdr:colOff>
+      <xdr:colOff>505800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1593,7 +1623,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1638720"/>
-          <a:ext cx="408240" cy="425160"/>
+          <a:ext cx="407880" cy="424800"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1685,9 +1715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>91800</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1697,7 +1727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4480920" y="1338120"/>
-          <a:ext cx="1078560" cy="742680"/>
+          <a:ext cx="1078200" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1770,9 +1800,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>624600</xdr:colOff>
+      <xdr:colOff>624240</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1782,7 +1812,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734080" y="5127120"/>
-          <a:ext cx="1212480" cy="628920"/>
+          <a:ext cx="1212120" cy="628560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1860,9 +1890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>396720</xdr:colOff>
+      <xdr:colOff>396360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1871,7 +1901,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1480680"/>
-        <a:ext cx="4808880" cy="2665440"/>
+        <a:ext cx="4808520" cy="2665080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1891,8 +1921,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2384,7 +2414,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K38" activeCellId="0" sqref="K38"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2587,7 +2617,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2632,7 +2662,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>41921</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">Sprint1!G12</f>
+        <v>150</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">Sprint1!H12</f>
+        <v>580</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <f aca="false">(D3-D2)/E3</f>
+        <v>0.258620689655172</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2650,17 +2699,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="26.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.41"/>
@@ -2715,6 +2764,15 @@
       <c r="F2" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="G2" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -2732,6 +2790,15 @@
       <c r="F3" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -2749,6 +2816,15 @@
       <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -2766,6 +2842,15 @@
       <c r="F5" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -2783,6 +2868,15 @@
       <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2801,7 +2895,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>70</v>
@@ -2827,7 +2921,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>30</v>
@@ -2852,23 +2946,93 @@
       <c r="F9" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <f aca="false">SUM(G2:G9)</f>
+        <v>150</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">SUM(H2:H9)</f>
+        <v>580</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2885,15 +3049,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,6 +3091,137 @@
         <v>117</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3055,15 +3352,15 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="47.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="48.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -3081,22 +3378,22 @@
         <v>29</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
@@ -3104,7 +3401,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -3127,7 +3424,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -3150,7 +3447,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3173,7 +3470,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -3196,7 +3493,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -3219,7 +3516,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3243,7 +3540,7 @@
         <v>45</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -3266,7 +3563,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -3289,7 +3586,7 @@
         <v>49</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -3303,7 +3600,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -3311,13 +3608,13 @@
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,7 +3625,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -3336,13 +3633,13 @@
     </row>
     <row r="14" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3353,7 +3650,7 @@
         <v>55</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -3367,7 +3664,7 @@
         <v>57</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -3381,7 +3678,7 @@
         <v>59</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -3389,13 +3686,13 @@
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,35 +3703,35 @@
         <v>61</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,7 +3742,7 @@
         <v>63</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
@@ -3459,7 +3756,7 @@
         <v>65</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
@@ -3473,7 +3770,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
@@ -3481,13 +3778,13 @@
     </row>
     <row r="25" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,7 +3795,7 @@
         <v>69</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
@@ -3506,13 +3803,13 @@
     </row>
     <row r="27" customFormat="false" ht="130" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3820,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -3537,13 +3834,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,7 +3851,7 @@
         <v>75</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -3568,7 +3865,7 @@
         <v>77</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
@@ -3582,7 +3879,7 @@
         <v>79</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -3596,7 +3893,7 @@
         <v>81</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -3610,24 +3907,24 @@
         <v>83</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,7 +3935,7 @@
         <v>85</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
@@ -3652,7 +3949,7 @@
         <v>87</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -3666,7 +3963,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -3680,7 +3977,7 @@
         <v>91</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
@@ -3694,7 +3991,7 @@
         <v>93</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
@@ -3702,24 +3999,24 @@
     </row>
     <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,7 +4027,7 @@
         <v>95</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Add comments do us21 + update report
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -735,7 +735,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,6 +786,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -868,7 +872,224 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4a7ebb"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="4a7ebb"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4a7ebb"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burndown README'!$B$15:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6/6/2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6/19/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7/3/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7/17/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7/31/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown README'!$C$15:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="59480735"/>
+        <c:axId val="94417373"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="59480735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="M/D/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94417373"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="94417373"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59480735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -973,11 +1194,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="79595002"/>
-        <c:axId val="33890008"/>
+        <c:axId val="52376627"/>
+        <c:axId val="96879495"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79595002"/>
+        <c:axId val="52376627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,14 +1230,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33890008"/>
+        <c:crossAx val="96879495"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33890008"/>
+        <c:axId val="96879495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,224 +1279,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79595002"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Burndown README'!$B$15:$B$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>6/6/2016</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6/19/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7/3/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7/17/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7/31/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Burndown README'!$C$15:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:axId val="22440447"/>
-        <c:axId val="77433751"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="22440447"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="M/D/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="77433751"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="77433751"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="878787"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="22440447"/>
+        <c:crossAx val="52376627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1313,9 +1317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>395280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1324,7 +1328,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3628440"/>
-        <a:ext cx="4915080" cy="2667960"/>
+        <a:ext cx="4914720" cy="2667600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1343,9 +1347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>946080</xdr:colOff>
+      <xdr:colOff>945720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1355,7 +1359,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512000"/>
-          <a:ext cx="1242720" cy="627120"/>
+          <a:ext cx="1242360" cy="626760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1447,9 +1451,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>496440</xdr:colOff>
+      <xdr:colOff>496080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1459,7 +1463,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5581800" y="1486440"/>
-          <a:ext cx="1236600" cy="534240"/>
+          <a:ext cx="1236240" cy="533880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1532,9 +1536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>61200</xdr:colOff>
+      <xdr:colOff>60840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1544,7 +1548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2878920" y="1316520"/>
-          <a:ext cx="1091880" cy="797040"/>
+          <a:ext cx="1091520" cy="796680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1617,9 +1621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>505080</xdr:colOff>
+      <xdr:colOff>504720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1629,7 +1633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1638720"/>
-          <a:ext cx="407160" cy="424080"/>
+          <a:ext cx="406800" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1721,9 +1725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1733,7 +1737,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4480920" y="1338120"/>
-          <a:ext cx="1077480" cy="741600"/>
+          <a:ext cx="1077120" cy="741240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1806,9 +1810,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
+      <xdr:colOff>623160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1818,7 +1822,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734080" y="5127120"/>
-          <a:ext cx="1211400" cy="627840"/>
+          <a:ext cx="1211040" cy="627480"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1896,9 +1900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>395280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1907,7 +1911,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1480680"/>
-        <a:ext cx="4807800" cy="2664360"/>
+        <a:ext cx="4807440" cy="2664000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2779,7 +2783,7 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3145,15 +3149,17 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,6 +3325,12 @@
       </c>
       <c r="F9" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3328,6 +3340,10 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3506,7 +3522,7 @@
       <c r="B2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -3529,7 +3545,7 @@
       <c r="B3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -3552,7 +3568,7 @@
       <c r="B4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -3575,7 +3591,7 @@
       <c r="B5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>139</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -3598,7 +3614,7 @@
       <c r="B6" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -3621,7 +3637,7 @@
       <c r="B7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>141</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -3636,7 +3652,7 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -3645,7 +3661,7 @@
       <c r="B8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>142</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -3668,7 +3684,7 @@
       <c r="B9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>143</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -3691,7 +3707,7 @@
       <c r="B10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>144</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -3705,7 +3721,7 @@
       <c r="B11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>145</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -3719,7 +3735,7 @@
       <c r="B12" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3730,7 +3746,7 @@
       <c r="B13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -3744,7 +3760,7 @@
       <c r="B14" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3755,7 +3771,7 @@
       <c r="B15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>153</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -3769,7 +3785,7 @@
       <c r="B16" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>154</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -3783,7 +3799,7 @@
       <c r="B17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>155</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -3797,7 +3813,7 @@
       <c r="B18" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3808,7 +3824,7 @@
       <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -3825,7 +3841,7 @@
       <c r="B20" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3836,7 +3852,7 @@
       <c r="B21" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="14" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3847,7 +3863,7 @@
       <c r="B22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>167</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -3861,7 +3877,7 @@
       <c r="B23" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>168</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -3875,7 +3891,7 @@
       <c r="B24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>169</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -3889,7 +3905,7 @@
       <c r="B25" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="14" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3900,7 +3916,7 @@
       <c r="B26" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>173</v>
       </c>
       <c r="D26" s="0" t="n">
@@ -3914,7 +3930,7 @@
       <c r="B27" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3925,7 +3941,7 @@
       <c r="B28" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D28" s="0" t="n">
@@ -3939,7 +3955,7 @@
       <c r="B29" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="14" t="s">
         <v>178</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3956,7 +3972,7 @@
       <c r="B30" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="14" t="s">
         <v>179</v>
       </c>
       <c r="D30" s="0" t="n">
@@ -3970,7 +3986,7 @@
       <c r="B31" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="14" t="s">
         <v>180</v>
       </c>
       <c r="D31" s="0" t="n">
@@ -3984,7 +4000,7 @@
       <c r="B32" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="14" t="s">
         <v>181</v>
       </c>
       <c r="D32" s="0" t="n">
@@ -3998,7 +4014,7 @@
       <c r="B33" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>182</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -4012,7 +4028,7 @@
       <c r="B34" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>183</v>
       </c>
       <c r="D34" s="0" t="n">
@@ -4029,7 +4045,7 @@
       <c r="B35" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4040,7 +4056,7 @@
       <c r="B36" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>187</v>
       </c>
       <c r="D36" s="0" t="n">
@@ -4054,7 +4070,7 @@
       <c r="B37" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="14" t="s">
         <v>188</v>
       </c>
       <c r="D37" s="0" t="n">
@@ -4068,7 +4084,7 @@
       <c r="B38" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>189</v>
       </c>
       <c r="D38" s="0" t="n">
@@ -4082,7 +4098,7 @@
       <c r="B39" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>190</v>
       </c>
       <c r="D39" s="0" t="n">
@@ -4096,7 +4112,7 @@
       <c r="B40" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>191</v>
       </c>
       <c r="D40" s="0" t="n">
@@ -4110,7 +4126,7 @@
       <c r="B41" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4121,7 +4137,7 @@
       <c r="B42" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="14" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4132,7 +4148,7 @@
       <c r="B43" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>198</v>
       </c>
       <c r="D43" s="0" t="n">

</xml_diff>

<commit_message>
Add comment + update report
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -639,12 +639,11 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -663,10 +662,86 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -684,10 +759,9 @@
       <sz val="12"/>
       <name val="Cambria"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,12 +770,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF878787"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD7E4BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -709,8 +825,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -734,13 +865,64 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -752,11 +934,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,11 +946,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,23 +958,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,32 +979,49 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FFD7E4BD"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -834,7 +1029,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -845,12 +1040,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFD7E4BD"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -858,7 +1053,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF4A7EBB"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF878787"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -872,7 +1067,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -977,11 +1172,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="59480735"/>
-        <c:axId val="94417373"/>
+        <c:axId val="97084921"/>
+        <c:axId val="34302637"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59480735"/>
+        <c:axId val="97084921"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,14 +1208,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94417373"/>
+        <c:crossAx val="34302637"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94417373"/>
+        <c:axId val="34302637"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1257,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59480735"/>
+        <c:crossAx val="97084921"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1089,7 +1284,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1194,11 +1389,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="52376627"/>
-        <c:axId val="96879495"/>
+        <c:axId val="95097469"/>
+        <c:axId val="25320551"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52376627"/>
+        <c:axId val="95097469"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,14 +1425,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96879495"/>
+        <c:crossAx val="25320551"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96879495"/>
+        <c:axId val="25320551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1474,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52376627"/>
+        <c:crossAx val="95097469"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1313,13 +1508,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>75240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395280</xdr:colOff>
+      <xdr:colOff>395640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1327,8 +1522,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="948240" y="3628440"/>
-        <a:ext cx="4914720" cy="2667600"/>
+        <a:off x="948240" y="3629160"/>
+        <a:ext cx="4915080" cy="2666520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1343,13 +1538,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>469080</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>945720</xdr:colOff>
+      <xdr:colOff>946080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1358,8 +1553,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1342080" y="1512000"/>
-          <a:ext cx="1242360" cy="626760"/>
+          <a:off x="1342080" y="1512720"/>
+          <a:ext cx="1242720" cy="625680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1385,7 +1580,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1445,15 +1640,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>114840</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>496080</xdr:colOff>
+      <xdr:colOff>495720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1462,8 +1657,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581800" y="1486440"/>
-          <a:ext cx="1236240" cy="533880"/>
+          <a:off x="5582520" y="1487160"/>
+          <a:ext cx="1235160" cy="532800"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1489,7 +1684,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1530,15 +1725,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1240200</xdr:colOff>
+      <xdr:colOff>1240920</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>60840</xdr:colOff>
+      <xdr:colOff>60480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1547,8 +1742,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2878920" y="1316520"/>
-          <a:ext cx="1091520" cy="796680"/>
+          <a:off x="2879640" y="1316520"/>
+          <a:ext cx="1090440" cy="796320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1574,7 +1769,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1617,13 +1812,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>97920</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>504720</xdr:colOff>
+      <xdr:colOff>504360</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1632,8 +1827,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4007520" y="1638720"/>
-          <a:ext cx="406800" cy="423720"/>
+          <a:off x="4007520" y="1639440"/>
+          <a:ext cx="406440" cy="422640"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1659,7 +1854,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1719,15 +1914,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>20880</xdr:colOff>
+      <xdr:colOff>21600</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90360</xdr:colOff>
+      <xdr:colOff>90720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1736,8 +1931,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4480920" y="1338120"/>
-          <a:ext cx="1077120" cy="741240"/>
+          <a:off x="4481640" y="1338840"/>
+          <a:ext cx="1076760" cy="740160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1763,7 +1958,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1804,15 +1999,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>266400</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>623160</xdr:colOff>
+      <xdr:colOff>622800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1821,8 +2016,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5734080" y="5127120"/>
-          <a:ext cx="1211040" cy="627480"/>
+          <a:off x="5734800" y="5127840"/>
+          <a:ext cx="1209960" cy="627120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1848,7 +2043,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dir="5400000" dist="23040">
+          <a:outerShdw dist="23040" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1900,9 +2095,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395280</xdr:colOff>
+      <xdr:colOff>395640</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1911,7 +2106,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1480680"/>
-        <a:ext cx="4807440" cy="2664000"/>
+        <a:ext cx="4807800" cy="2663640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2784,7 +2979,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3150,7 +3345,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3309,6 +3504,12 @@
       <c r="F8" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -3329,7 +3530,7 @@
       <c r="G9" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="n">
+      <c r="H9" s="0" t="n">
         <v>120</v>
       </c>
     </row>
@@ -3522,7 +3723,7 @@
       <c r="B2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -3545,7 +3746,7 @@
       <c r="B3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -3568,7 +3769,7 @@
       <c r="B4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -3591,7 +3792,7 @@
       <c r="B5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>139</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -3614,7 +3815,7 @@
       <c r="B6" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -3637,7 +3838,7 @@
       <c r="B7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>141</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -3652,7 +3853,7 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -3661,7 +3862,7 @@
       <c r="B8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>142</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -3684,7 +3885,7 @@
       <c r="B9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>143</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -3707,7 +3908,7 @@
       <c r="B10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>144</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -3721,7 +3922,7 @@
       <c r="B11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>145</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -3735,7 +3936,7 @@
       <c r="B12" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3746,7 +3947,7 @@
       <c r="B13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -3760,7 +3961,7 @@
       <c r="B14" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3771,7 +3972,7 @@
       <c r="B15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>153</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -3785,7 +3986,7 @@
       <c r="B16" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>154</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -3799,7 +4000,7 @@
       <c r="B17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>155</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -3813,7 +4014,7 @@
       <c r="B18" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3824,7 +4025,7 @@
       <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -3841,7 +4042,7 @@
       <c r="B20" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3852,7 +4053,7 @@
       <c r="B21" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3863,7 +4064,7 @@
       <c r="B22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>167</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -3877,7 +4078,7 @@
       <c r="B23" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>168</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -3891,7 +4092,7 @@
       <c r="B24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>169</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -3905,7 +4106,7 @@
       <c r="B25" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3916,7 +4117,7 @@
       <c r="B26" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>173</v>
       </c>
       <c r="D26" s="0" t="n">
@@ -3930,7 +4131,7 @@
       <c r="B27" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3941,7 +4142,7 @@
       <c r="B28" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>177</v>
       </c>
       <c r="D28" s="0" t="n">
@@ -3955,7 +4156,7 @@
       <c r="B29" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>178</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3972,7 +4173,7 @@
       <c r="B30" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>179</v>
       </c>
       <c r="D30" s="0" t="n">
@@ -3986,7 +4187,7 @@
       <c r="B31" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D31" s="0" t="n">
@@ -4000,7 +4201,7 @@
       <c r="B32" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>181</v>
       </c>
       <c r="D32" s="0" t="n">
@@ -4014,7 +4215,7 @@
       <c r="B33" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>182</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -4028,7 +4229,7 @@
       <c r="B34" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>183</v>
       </c>
       <c r="D34" s="0" t="n">
@@ -4045,7 +4246,7 @@
       <c r="B35" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4056,7 +4257,7 @@
       <c r="B36" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>187</v>
       </c>
       <c r="D36" s="0" t="n">
@@ -4070,7 +4271,7 @@
       <c r="B37" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>188</v>
       </c>
       <c r="D37" s="0" t="n">
@@ -4084,7 +4285,7 @@
       <c r="B38" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>189</v>
       </c>
       <c r="D38" s="0" t="n">
@@ -4098,7 +4299,7 @@
       <c r="B39" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>190</v>
       </c>
       <c r="D39" s="0" t="n">
@@ -4112,7 +4313,7 @@
       <c r="B40" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>191</v>
       </c>
       <c r="D40" s="0" t="n">
@@ -4126,7 +4327,7 @@
       <c r="B41" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4137,7 +4338,7 @@
       <c r="B42" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4148,7 +4349,7 @@
       <c r="B43" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>198</v>
       </c>
       <c r="D43" s="0" t="n">

</xml_diff>

<commit_message>
Update report after sprint 2 review meeting
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="205">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -421,6 +421,24 @@
   </si>
   <si>
     <t xml:space="preserve">Bad / dirty code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling in for people who need help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Being patient with less experienced programmers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discuss stories shortly in sprint meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assign similar stories to the same person although they might be difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarcasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cz</t>
   </si>
   <si>
     <t xml:space="preserve">Story Description</t>
@@ -639,11 +657,12 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -662,86 +681,10 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -759,9 +702,10 @@
       <sz val="12"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -770,54 +714,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF878787"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD7E4BD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -825,23 +727,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -865,64 +752,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -934,11 +770,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,11 +782,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -958,20 +794,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -979,49 +823,32 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFD7E4BD"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF878787"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1029,7 +856,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1040,12 +867,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFD7E4BD"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1053,7 +880,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF4A7EBB"/>
-      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1067,7 +894,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1172,11 +999,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="97084921"/>
-        <c:axId val="34302637"/>
+        <c:axId val="15530130"/>
+        <c:axId val="20121339"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97084921"/>
+        <c:axId val="15530130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,14 +1035,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34302637"/>
+        <c:crossAx val="20121339"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34302637"/>
+        <c:axId val="20121339"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1084,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97084921"/>
+        <c:crossAx val="15530130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1284,7 +1111,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1338,7 +1165,7 @@
                   <c:v>10/10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>10/22</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1365,7 +1192,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1389,11 +1216,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="95097469"/>
-        <c:axId val="25320551"/>
+        <c:axId val="80693650"/>
+        <c:axId val="23272101"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95097469"/>
+        <c:axId val="80693650"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,14 +1252,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25320551"/>
+        <c:crossAx val="23272101"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25320551"/>
+        <c:axId val="23272101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1301,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95097469"/>
+        <c:crossAx val="80693650"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1512,9 +1339,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>395280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1523,7 +1350,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4915080" cy="2666520"/>
+        <a:ext cx="4914720" cy="2666160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1542,9 +1369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>946080</xdr:colOff>
+      <xdr:colOff>945720</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1554,7 +1381,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1242720" cy="625680"/>
+          <a:ext cx="1242360" cy="625320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1580,7 +1407,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1646,9 +1473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>495720</xdr:colOff>
+      <xdr:colOff>495360</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1658,7 +1485,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1235160" cy="532800"/>
+          <a:ext cx="1234800" cy="532440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1684,7 +1511,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1731,9 +1558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>60480</xdr:colOff>
+      <xdr:colOff>60120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1743,7 +1570,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1090440" cy="796320"/>
+          <a:ext cx="1090080" cy="795960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1769,7 +1596,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1816,9 +1643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>504360</xdr:colOff>
+      <xdr:colOff>504000</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1828,7 +1655,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="406440" cy="422640"/>
+          <a:ext cx="406080" cy="422280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1854,7 +1681,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1920,9 +1747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1932,7 +1759,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1076760" cy="740160"/>
+          <a:ext cx="1076400" cy="739800"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1958,7 +1785,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -2005,9 +1832,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>622800</xdr:colOff>
+      <xdr:colOff>622440</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2017,7 +1844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1209960" cy="627120"/>
+          <a:ext cx="1209600" cy="626760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2043,7 +1870,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw dist="23040" dir="5400000">
+          <a:outerShdw dir="5400000" dist="23040">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -2095,7 +1922,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
@@ -2105,8 +1932,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="948240" y="1480680"/>
-        <a:ext cx="4807800" cy="2663640"/>
+        <a:off x="948240" y="1470600"/>
+        <a:ext cx="4807800" cy="2663280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2126,7 +1953,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2251,7 +2078,7 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2690,7 +2517,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2891,16 +2718,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.83"/>
@@ -2929,8 +2756,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>40444</v>
+      <c r="A2" s="6" t="n">
+        <v>41905</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>32</v>
@@ -2940,7 +2767,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="6" t="n">
         <v>41921</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2959,6 +2786,29 @@
         <v>0.258620689655172</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>41933</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">D3+Sprint2!G12</f>
+        <v>372</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">E3+Sprint2!H12</f>
+        <v>1440</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <f aca="false">(D4-D3)/E4</f>
+        <v>0.154166666666667</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2978,8 +2828,8 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3342,16 +3192,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.59"/>
@@ -3396,11 +3246,23 @@
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3413,11 +3275,23 @@
       <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,11 +3304,23 @@
       <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E4" s="0" t="n">
         <v>20</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,11 +3333,23 @@
       <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E5" s="0" t="n">
         <v>25</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,11 +3362,23 @@
       <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,11 +3391,23 @@
       <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,6 +3420,9 @@
       <c r="C8" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="0" t="n">
         <v>30</v>
       </c>
@@ -3509,6 +3434,9 @@
       </c>
       <c r="H8" s="0" t="n">
         <v>80</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,6 +3449,9 @@
       <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E9" s="0" t="n">
         <v>20</v>
       </c>
@@ -3533,18 +3464,98 @@
       <c r="H9" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <f aca="false">SUM(G2:G9)</f>
+        <v>222</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">SUM(H2:H9)</f>
+        <v>860</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3561,18 +3572,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3601,6 +3614,144 @@
         <v>118</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3619,7 +3770,7 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3673,17 +3824,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="48.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -3693,30 +3844,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.32"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>131</v>
+      <c r="C1" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
@@ -3724,7 +3876,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -3739,7 +3891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>35</v>
       </c>
@@ -3747,7 +3899,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -3762,7 +3914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>37</v>
       </c>
@@ -3770,7 +3922,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3785,7 +3937,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>39</v>
       </c>
@@ -3793,7 +3945,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -3808,7 +3960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>41</v>
       </c>
@@ -3816,7 +3968,7 @@
         <v>42</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -3831,7 +3983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>43</v>
       </c>
@@ -3839,7 +3991,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3853,9 +4005,9 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>45</v>
       </c>
@@ -3863,7 +4015,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -3878,7 +4030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +4038,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -3901,7 +4053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>49</v>
       </c>
@@ -3909,13 +4061,13 @@
         <v>50</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>51</v>
       </c>
@@ -3923,24 +4075,24 @@
         <v>52</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>53</v>
       </c>
@@ -3948,24 +4100,24 @@
         <v>54</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>55</v>
       </c>
@@ -3973,13 +4125,13 @@
         <v>56</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>57</v>
       </c>
@@ -3987,13 +4139,13 @@
         <v>58</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>59</v>
       </c>
@@ -4001,21 +4153,21 @@
         <v>60</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4026,38 +4178,38 @@
         <v>62</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>63</v>
       </c>
@@ -4065,13 +4217,13 @@
         <v>64</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>65</v>
       </c>
@@ -4079,13 +4231,13 @@
         <v>66</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>67</v>
       </c>
@@ -4093,24 +4245,24 @@
         <v>68</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>69</v>
       </c>
@@ -4118,24 +4270,24 @@
         <v>70</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="130" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>71</v>
       </c>
@@ -4143,13 +4295,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>73</v>
       </c>
@@ -4157,13 +4309,13 @@
         <v>74</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4174,7 +4326,7 @@
         <v>76</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -4188,13 +4340,13 @@
         <v>78</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>79</v>
       </c>
@@ -4202,7 +4354,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -4216,13 +4368,13 @@
         <v>82</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>83</v>
       </c>
@@ -4230,27 +4382,27 @@
         <v>84</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>85</v>
       </c>
@@ -4258,13 +4410,13 @@
         <v>86</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>87</v>
       </c>
@@ -4272,13 +4424,13 @@
         <v>88</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>89</v>
       </c>
@@ -4286,13 +4438,13 @@
         <v>90</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>91</v>
       </c>
@@ -4300,13 +4452,13 @@
         <v>92</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>93</v>
       </c>
@@ -4314,35 +4466,35 @@
         <v>94</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>95</v>
       </c>
@@ -4350,7 +4502,7 @@
         <v>96</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Implement US 28 - Order siblings by age
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -753,7 +753,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -808,6 +808,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -894,7 +898,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -999,11 +1003,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="39257461"/>
-        <c:axId val="35203312"/>
+        <c:axId val="31911442"/>
+        <c:axId val="39713211"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39257461"/>
+        <c:axId val="31911442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,14 +1039,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35203312"/>
+        <c:crossAx val="39713211"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35203312"/>
+        <c:axId val="39713211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1088,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39257461"/>
+        <c:crossAx val="31911442"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1111,7 +1115,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1216,11 +1220,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="65189566"/>
-        <c:axId val="30503738"/>
+        <c:axId val="37383141"/>
+        <c:axId val="38114344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65189566"/>
+        <c:axId val="37383141"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,14 +1256,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30503738"/>
+        <c:crossAx val="38114344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30503738"/>
+        <c:axId val="38114344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,7 +1305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65189566"/>
+        <c:crossAx val="37383141"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1339,9 +1343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>394920</xdr:colOff>
+      <xdr:colOff>394200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1350,7 +1354,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4914360" cy="2665800"/>
+        <a:ext cx="4913640" cy="2665080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1369,9 +1373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>945360</xdr:colOff>
+      <xdr:colOff>944640</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1381,7 +1385,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1242000" cy="624960"/>
+          <a:ext cx="1241280" cy="624240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1473,9 +1477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>495000</xdr:colOff>
+      <xdr:colOff>494280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1485,7 +1489,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1234440" cy="532080"/>
+          <a:ext cx="1233720" cy="531360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1558,9 +1562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>59760</xdr:colOff>
+      <xdr:colOff>59040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1570,7 +1574,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1089720" cy="795600"/>
+          <a:ext cx="1089000" cy="794880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1643,9 +1647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>503640</xdr:colOff>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1655,7 +1659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="405720" cy="421920"/>
+          <a:ext cx="405000" cy="421200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1747,9 +1751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1759,7 +1763,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1076040" cy="739440"/>
+          <a:ext cx="1075320" cy="738720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1832,9 +1836,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>622080</xdr:colOff>
+      <xdr:colOff>621360</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1844,7 +1848,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1209240" cy="626400"/>
+          <a:ext cx="1208520" cy="625680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1922,9 +1926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1933,7 +1937,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4807440" cy="2662920"/>
+        <a:ext cx="4806720" cy="2662200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1953,7 +1957,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2078,7 +2082,7 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -2590,7 +2594,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2793,7 +2797,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -2901,7 +2905,7 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3267,7 +3271,7 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3647,15 +3651,17 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,6 +3759,12 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3855,7 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3899,15 +3911,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="63.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -3924,7 +3936,7 @@
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4078,7 +4090,7 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">

</xml_diff>

<commit_message>
Complete US 27 - include individuals age #33
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -753,7 +753,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -808,6 +808,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -999,11 +1003,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="72546053"/>
-        <c:axId val="28209402"/>
+        <c:axId val="14701451"/>
+        <c:axId val="88750261"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72546053"/>
+        <c:axId val="14701451"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,14 +1039,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28209402"/>
+        <c:crossAx val="88750261"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28209402"/>
+        <c:axId val="88750261"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1088,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72546053"/>
+        <c:crossAx val="14701451"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1216,11 +1220,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="64646809"/>
-        <c:axId val="90183798"/>
+        <c:axId val="13563790"/>
+        <c:axId val="58730648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64646809"/>
+        <c:axId val="13563790"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,14 +1256,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90183798"/>
+        <c:crossAx val="58730648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90183798"/>
+        <c:axId val="58730648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,7 +1305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64646809"/>
+        <c:crossAx val="13563790"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1339,9 +1343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>393840</xdr:colOff>
+      <xdr:colOff>393480</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1350,7 +1354,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4913280" cy="2664720"/>
+        <a:ext cx="4912920" cy="2664360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1369,9 +1373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>944280</xdr:colOff>
+      <xdr:colOff>943920</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1381,7 +1385,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1240920" cy="623880"/>
+          <a:ext cx="1240560" cy="623520"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1473,9 +1477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>493920</xdr:colOff>
+      <xdr:colOff>493560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1485,7 +1489,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1233360" cy="531000"/>
+          <a:ext cx="1233000" cy="530640"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1558,9 +1562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>58680</xdr:colOff>
+      <xdr:colOff>58320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1570,7 +1574,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1088640" cy="794520"/>
+          <a:ext cx="1088280" cy="794160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1643,9 +1647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>502560</xdr:colOff>
+      <xdr:colOff>502200</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1655,7 +1659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="404640" cy="420840"/>
+          <a:ext cx="404280" cy="420480"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1747,9 +1751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>88920</xdr:colOff>
+      <xdr:colOff>88560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1759,7 +1763,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1074960" cy="738360"/>
+          <a:ext cx="1074600" cy="738000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1832,9 +1836,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>621000</xdr:colOff>
+      <xdr:colOff>620640</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1844,7 +1848,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1208160" cy="625320"/>
+          <a:ext cx="1207800" cy="624960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1922,9 +1926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>237960</xdr:colOff>
+      <xdr:colOff>237600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1933,7 +1937,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4806360" cy="2661840"/>
+        <a:ext cx="4806000" cy="2661480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3655,8 +3659,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="10.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.59"/>
   </cols>
   <sheetData>
@@ -3756,11 +3760,11 @@
       <c r="F5" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>25</v>
+      <c r="G5" s="14" t="n">
+        <v>5</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3777,6 +3781,12 @@
         <v>40</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>90</v>
       </c>
     </row>
@@ -3915,7 +3925,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="63.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -3932,7 +3942,7 @@
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4086,7 +4096,7 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">

</xml_diff>

<commit_message>
Plan sprint 4 + add readme sprint 3
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="206">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -441,6 +441,33 @@
     <t xml:space="preserve">cz</t>
   </si>
   <si>
+    <t xml:space="preserve">List all multiple births in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all people in a GEDCOM file who were born in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract day, month → compare todays day, month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Story Description</t>
   </si>
   <si>
@@ -594,12 +621,6 @@
     <t xml:space="preserve">List all living people over 30 who have never been married in a GEDCOM file</t>
   </si>
   <si>
-    <t xml:space="preserve">List all multiple births in a GEDCOM file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
-  </si>
-  <si>
     <t xml:space="preserve">US34</t>
   </si>
   <si>
@@ -609,21 +630,6 @@
     <t xml:space="preserve">List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
   </si>
   <si>
-    <t xml:space="preserve">List all people in a GEDCOM file who were born in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
-  </si>
-  <si>
     <t xml:space="preserve">US40</t>
   </si>
   <si>
@@ -640,9 +646,6 @@
   </si>
   <si>
     <t xml:space="preserve">Accept and use dates without days or without days and months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -810,8 +813,12 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -898,7 +905,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1003,11 +1010,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="14701451"/>
-        <c:axId val="88750261"/>
+        <c:axId val="69183332"/>
+        <c:axId val="97199668"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14701451"/>
+        <c:axId val="69183332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1039,14 +1046,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88750261"/>
+        <c:crossAx val="97199668"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88750261"/>
+        <c:axId val="97199668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14701451"/>
+        <c:crossAx val="69183332"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1115,7 +1122,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1172,7 +1179,7 @@
                   <c:v>10/22/2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>11/7/2018</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v/>
@@ -1199,7 +1206,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v/>
@@ -1220,11 +1227,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="13563790"/>
-        <c:axId val="58730648"/>
+        <c:axId val="92835749"/>
+        <c:axId val="61451438"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13563790"/>
+        <c:axId val="92835749"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,14 +1263,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58730648"/>
+        <c:crossAx val="61451438"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58730648"/>
+        <c:axId val="61451438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1312,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13563790"/>
+        <c:crossAx val="92835749"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1343,9 +1350,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>393480</xdr:colOff>
+      <xdr:colOff>392760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1354,7 +1361,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4912920" cy="2664360"/>
+        <a:ext cx="4912200" cy="2663640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1373,9 +1380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>943920</xdr:colOff>
+      <xdr:colOff>943200</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1385,7 +1392,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1240560" cy="623520"/>
+          <a:ext cx="1239840" cy="622800"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1477,9 +1484,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
+      <xdr:colOff>492840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1489,7 +1496,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1233000" cy="530640"/>
+          <a:ext cx="1232280" cy="529920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1562,9 +1569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>57600</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1574,7 +1581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1088280" cy="794160"/>
+          <a:ext cx="1087560" cy="793440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1647,9 +1654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>502200</xdr:colOff>
+      <xdr:colOff>501480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1659,7 +1666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="404280" cy="420480"/>
+          <a:ext cx="403560" cy="419760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1751,9 +1758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
+      <xdr:colOff>87840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1763,7 +1770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1074600" cy="738000"/>
+          <a:ext cx="1073880" cy="737280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1836,9 +1843,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>620640</xdr:colOff>
+      <xdr:colOff>619920</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1848,7 +1855,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1207800" cy="624960"/>
+          <a:ext cx="1207080" cy="624240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1926,9 +1933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>237600</xdr:colOff>
+      <xdr:colOff>236880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1937,7 +1944,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4806000" cy="2661480"/>
+        <a:ext cx="4805280" cy="2660760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1957,7 +1964,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2082,7 +2089,7 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -2594,7 +2601,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2795,10 +2802,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2883,7 +2890,26 @@
         <v>0.154166666666667</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>41949</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">D4+Sprint3!G12</f>
+        <v>526</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">E4+Sprint3!H12</f>
+        <v>1770</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <f aca="false">(D5-D4)/E5</f>
+        <v>0.0870056497175141</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2905,7 +2931,7 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3271,8 +3297,8 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3649,10 +3675,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3703,11 +3729,23 @@
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" s="0" t="n">
         <v>37</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,11 +3758,23 @@
       <c r="C3" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3737,11 +3787,23 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E4" s="0" t="n">
         <v>45</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,17 +3816,23 @@
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E5" s="0" t="n">
         <v>15</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3777,6 +3845,9 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="0" t="n">
         <v>40</v>
       </c>
@@ -3788,6 +3859,9 @@
       </c>
       <c r="H6" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,11 +3874,23 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,11 +3903,23 @@
       <c r="C8" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="0" t="n">
         <v>40</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,15 +3932,44 @@
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E9" s="0" t="n">
         <v>15</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <f aca="false">SUM(G2:G9)</f>
+        <v>154</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">SUM(H2:H9)</f>
+        <v>330</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3859,46 +3986,219 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>118</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3917,15 +4217,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="63.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -3942,20 +4242,20 @@
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>137</v>
+      <c r="C1" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -3967,7 +4267,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -3990,7 +4290,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -4013,7 +4313,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -4036,7 +4336,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -4059,7 +4359,7 @@
         <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -4082,7 +4382,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -4096,7 +4396,7 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -4106,7 +4406,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -4129,7 +4429,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -4152,7 +4452,7 @@
         <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -4166,7 +4466,7 @@
         <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -4174,13 +4474,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4191,7 +4491,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -4199,13 +4499,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,7 +4516,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -4230,7 +4530,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -4244,7 +4544,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -4252,13 +4552,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,35 +4569,35 @@
         <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,7 +4608,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
@@ -4322,7 +4622,7 @@
         <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
@@ -4336,7 +4636,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
@@ -4344,13 +4644,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,7 +4661,7 @@
         <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
@@ -4369,13 +4669,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4386,7 +4686,7 @@
         <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -4400,13 +4700,13 @@
         <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4417,7 +4717,7 @@
         <v>76</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -4431,7 +4731,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
@@ -4445,7 +4745,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -4459,7 +4759,7 @@
         <v>82</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -4473,24 +4773,24 @@
         <v>84</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4501,7 +4801,7 @@
         <v>86</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
@@ -4515,7 +4815,7 @@
         <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>140</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -4529,7 +4829,7 @@
         <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -4543,7 +4843,7 @@
         <v>92</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
@@ -4557,7 +4857,7 @@
         <v>94</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
@@ -4565,24 +4865,24 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4593,7 +4893,7 @@
         <v>96</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>204</v>
+        <v>145</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
working on us42, incomplete and kinda broken
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="211">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -105,6 +105,21 @@
     <t xml:space="preserve">gruberma</t>
   </si>
   <si>
+    <t xml:space="preserve">cp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caroline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palicz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpalicz@stevens.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carlypalicz</t>
+  </si>
+  <si>
     <t xml:space="preserve">GitHub Repository:</t>
   </si>
   <si>
@@ -468,6 +483,24 @@
     <t xml:space="preserve">All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
   </si>
   <si>
+    <t xml:space="preserve">US11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No bigamy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage should not occur during marriage to another spouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siblings spacing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Story Description</t>
   </si>
   <si>
@@ -513,25 +546,7 @@
     <t xml:space="preserve">Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
   </si>
   <si>
-    <t xml:space="preserve">US11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No bigamy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siblings spacing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
   </si>
   <si>
     <t xml:space="preserve">No more than five siblings should be born at the same time</t>
@@ -660,7 +675,7 @@
     <numFmt numFmtId="168" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="169" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -685,6 +700,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Verdana"/>
       <family val="0"/>
       <charset val="1"/>
@@ -756,7 +778,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -765,7 +787,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -901,7 +927,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1006,11 +1032,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="16812139"/>
-        <c:axId val="34731138"/>
+        <c:axId val="81234050"/>
+        <c:axId val="41233526"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="16812139"/>
+        <c:axId val="81234050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,14 +1068,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34731138"/>
+        <c:crossAx val="41233526"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34731138"/>
+        <c:axId val="41233526"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1117,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16812139"/>
+        <c:crossAx val="81234050"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1118,7 +1144,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1223,11 +1249,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="77040925"/>
-        <c:axId val="18363738"/>
+        <c:axId val="35786682"/>
+        <c:axId val="31576412"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77040925"/>
+        <c:axId val="35786682"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,14 +1285,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18363738"/>
+        <c:crossAx val="31576412"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18363738"/>
+        <c:axId val="31576412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1334,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77040925"/>
+        <c:crossAx val="35786682"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1346,9 +1372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>392400</xdr:colOff>
+      <xdr:colOff>392040</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1357,7 +1383,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4911840" cy="2663280"/>
+        <a:ext cx="4911480" cy="2662920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1376,9 +1402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>942840</xdr:colOff>
+      <xdr:colOff>942480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1388,7 +1414,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1239480" cy="622440"/>
+          <a:ext cx="1239120" cy="622080"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1480,9 +1506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>492480</xdr:colOff>
+      <xdr:colOff>492120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1492,7 +1518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1231920" cy="529560"/>
+          <a:ext cx="1231560" cy="529200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1565,9 +1591,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>57240</xdr:colOff>
+      <xdr:colOff>56880</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1577,7 +1603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1087200" cy="793080"/>
+          <a:ext cx="1086840" cy="792720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1650,9 +1676,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>501120</xdr:colOff>
+      <xdr:colOff>500760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1662,7 +1688,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="403200" cy="419400"/>
+          <a:ext cx="402840" cy="419040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1754,9 +1780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1766,7 +1792,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1073520" cy="736920"/>
+          <a:ext cx="1073160" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1839,9 +1865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>619560</xdr:colOff>
+      <xdr:colOff>619200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1851,7 +1877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1206720" cy="623880"/>
+          <a:ext cx="1206360" cy="623520"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1929,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>236160</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1940,7 +1966,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4804920" cy="2660400"/>
+        <a:ext cx="4804560" cy="2660040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2058,16 +2084,36 @@
         <v>24</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="cpalicz@stevens.edu"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2086,7 +2132,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2101,19 +2147,19 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,16 +2167,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,16 +2184,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,16 +2201,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,16 +2218,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,16 +2235,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,16 +2252,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,16 +2269,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,16 +2286,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,16 +2303,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,16 +2320,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,16 +2337,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,16 +2354,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,16 +2371,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,16 +2388,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,16 +2405,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,16 +2422,16 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,13 +2439,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,13 +2456,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,13 +2473,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,13 +2490,16 @@
         <v>3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,13 +2507,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,13 +2524,16 @@
         <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,13 +2541,16 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,79 +2558,106 @@
         <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E25" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B26" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B27" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B28" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B29" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B30" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B32" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B33" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="L33" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="L33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2603,180 +2697,180 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>97</v>
+      <c r="A1" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>98</v>
+      <c r="A2" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>99</v>
+      <c r="A3" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>100</v>
+      <c r="A5" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>101</v>
+      <c r="A6" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>102</v>
+      <c r="A8" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>103</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="7" t="n">
+      <c r="A15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="8" t="n">
         <v>41065</v>
       </c>
-      <c r="C15" s="8" t="n">
+      <c r="C15" s="9" t="n">
         <v>24</v>
       </c>
-      <c r="E15" s="8" t="n">
+      <c r="E15" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="7" t="n">
+      <c r="A16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="8" t="n">
         <v>41078</v>
       </c>
-      <c r="C16" s="8" t="n">
+      <c r="C16" s="9" t="n">
         <v>18</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="8" t="n">
+      <c r="E16" s="9" t="n">
         <v>250</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="5" t="n">
         <f aca="false">(E16-E15)/F16*60</f>
         <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="7" t="n">
+      <c r="A17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="8" t="n">
         <v>41092</v>
       </c>
-      <c r="C17" s="8" t="n">
+      <c r="C17" s="9" t="n">
         <v>12</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="8" t="n">
+      <c r="E17" s="9" t="n">
         <v>480</v>
       </c>
-      <c r="F17" s="9" t="n">
+      <c r="F17" s="10" t="n">
         <v>135</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="5" t="n">
         <f aca="false">(E17-E16)/F17*60</f>
         <v>102.222222222222</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="7" t="n">
+      <c r="A18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="8" t="n">
         <v>41106</v>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="8" t="n">
+      <c r="E18" s="9" t="n">
         <v>740</v>
       </c>
-      <c r="F18" s="9" t="n">
+      <c r="F18" s="10" t="n">
         <v>160</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="5" t="n">
         <f aca="false">(E18-E17)/F18*60</f>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="7" t="n">
+      <c r="A19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="8" t="n">
         <v>41120</v>
       </c>
-      <c r="C19" s="8" t="n">
+      <c r="C19" s="9" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">C18-C19</f>
         <v>6</v>
       </c>
-      <c r="E19" s="8" t="n">
+      <c r="E19" s="9" t="n">
         <v>1100</v>
       </c>
-      <c r="F19" s="9" t="n">
+      <c r="F19" s="10" t="n">
         <v>145</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="5" t="n">
         <f aca="false">(E19-E18)/F19*60</f>
         <v>148.965517241379</v>
       </c>
@@ -2806,37 +2900,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>103</v>
+      <c r="A1" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="8" t="n">
         <v>41905</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -2847,7 +2941,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="8" t="n">
         <v>41921</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2861,13 +2955,13 @@
         <f aca="false">Sprint1!H12</f>
         <v>580</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="5" t="n">
         <f aca="false">(D3-D2)/E3</f>
         <v>0.258620689655172</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="8" t="n">
         <v>41933</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2881,13 +2975,13 @@
         <f aca="false">E3+Sprint2!H12</f>
         <v>1440</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <f aca="false">(D4-D3)/E4</f>
         <v>0.154166666666667</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="8" t="n">
         <v>41949</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -2901,7 +2995,7 @@
         <f aca="false">E4+Sprint3!H12</f>
         <v>1770</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <f aca="false">(D5-D4)/E5</f>
         <v>0.0870056497175141</v>
       </c>
@@ -2934,58 +3028,58 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>118</v>
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>15</v>
@@ -2999,22 +3093,22 @@
       <c r="H2" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>119</v>
+      <c r="I2" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
@@ -3028,22 +3122,22 @@
       <c r="H3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>119</v>
+      <c r="I3" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>30</v>
@@ -3057,22 +3151,22 @@
       <c r="H4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>119</v>
+      <c r="I4" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>30</v>
@@ -3086,22 +3180,22 @@
       <c r="H5" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>119</v>
+      <c r="I5" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>30</v>
@@ -3115,22 +3209,22 @@
       <c r="H6" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>119</v>
+      <c r="I6" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>15</v>
@@ -3144,22 +3238,22 @@
       <c r="H7" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>119</v>
+      <c r="I7" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>15</v>
@@ -3173,22 +3267,22 @@
       <c r="H8" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>119</v>
+      <c r="I8" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>45</v>
@@ -3202,16 +3296,16 @@
       <c r="H9" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>119</v>
+      <c r="I9" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,54 +3319,54 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="s">
-        <v>122</v>
+      <c r="B14" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
-        <v>124</v>
+      <c r="B18" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="s">
-        <v>125</v>
+      <c r="B19" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="s">
-        <v>126</v>
+      <c r="B20" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="11" t="s">
-        <v>128</v>
+      <c r="B23" s="12" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="s">
-        <v>129</v>
+      <c r="B25" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10" t="s">
-        <v>130</v>
+      <c r="B26" s="11" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3308,45 +3402,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>118</v>
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>30</v>
@@ -3360,22 +3454,22 @@
       <c r="H2" s="0" t="n">
         <v>240</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>119</v>
+      <c r="I2" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
@@ -3389,22 +3483,22 @@
       <c r="H3" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>119</v>
+      <c r="I3" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>20</v>
@@ -3418,22 +3512,22 @@
       <c r="H4" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>119</v>
+      <c r="I4" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>25</v>
@@ -3447,22 +3541,22 @@
       <c r="H5" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>119</v>
+      <c r="I5" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>30</v>
@@ -3476,22 +3570,22 @@
       <c r="H6" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>119</v>
+      <c r="I6" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>30</v>
@@ -3505,22 +3599,22 @@
       <c r="H7" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>119</v>
+      <c r="I7" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>30</v>
@@ -3534,22 +3628,22 @@
       <c r="H8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>119</v>
+      <c r="I8" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>20</v>
@@ -3563,17 +3657,17 @@
       <c r="H9" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>119</v>
+      <c r="I9" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3588,71 +3682,71 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="s">
-        <v>122</v>
+      <c r="B14" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
-        <v>124</v>
+      <c r="B18" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="s">
-        <v>125</v>
+      <c r="B19" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="s">
-        <v>126</v>
+      <c r="B20" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10" t="s">
-        <v>132</v>
+      <c r="B23" s="11" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="12" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="11" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="10" t="s">
-        <v>134</v>
+      <c r="B28" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="s">
-        <v>135</v>
+      <c r="B29" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3767,7 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -3688,45 +3782,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>118</v>
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>37</v>
@@ -3741,21 +3835,21 @@
         <v>60</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>73</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
@@ -3770,21 +3864,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>45</v>
@@ -3799,21 +3893,21 @@
         <v>60</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>15</v>
@@ -3828,21 +3922,21 @@
         <v>10</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>40</v>
@@ -3857,21 +3951,21 @@
         <v>90</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>15</v>
@@ -3886,21 +3980,21 @@
         <v>30</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>136</v>
+        <v>83</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>40</v>
@@ -3915,21 +4009,21 @@
         <v>30</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>15</v>
@@ -3944,15 +4038,15 @@
         <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,74 +4060,74 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="s">
-        <v>122</v>
+      <c r="B14" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
-        <v>124</v>
+      <c r="B18" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="s">
-        <v>125</v>
+      <c r="B19" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="s">
-        <v>126</v>
+      <c r="B20" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10" t="s">
-        <v>132</v>
+      <c r="B23" s="11" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="s">
-        <v>134</v>
+      <c r="B29" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="s">
-        <v>135</v>
+      <c r="B30" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4052,10 +4146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4068,43 +4162,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="12"/>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>118</v>
+        <v>36</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>20</v>
@@ -4118,13 +4212,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>89</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
@@ -4138,13 +4232,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>140</v>
+        <v>91</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>15</v>
@@ -4158,13 +4252,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>93</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>15</v>
@@ -4178,13 +4272,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>142</v>
+        <v>94</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>20</v>
@@ -4198,16 +4292,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>143</v>
+        <v>97</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>25</v>
@@ -4218,16 +4312,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>144</v>
+        <v>99</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>25</v>
@@ -4238,13 +4332,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>145</v>
+        <v>101</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
@@ -4256,8 +4350,46 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4277,15 +4409,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="63.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.25"/>
@@ -4297,37 +4429,37 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>146</v>
+        <v>34</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -4344,13 +4476,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -4367,13 +4499,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>153</v>
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -4390,13 +4522,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -4413,13 +4545,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -4436,13 +4568,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>156</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -4456,17 +4588,17 @@
       <c r="G7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>157</v>
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -4483,13 +4615,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>158</v>
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -4506,13 +4638,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>159</v>
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -4520,13 +4652,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>160</v>
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -4534,24 +4666,30 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>163</v>
+        <v>152</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>164</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -4559,24 +4697,30 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>168</v>
+        <v>61</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -4584,13 +4728,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>169</v>
+        <v>63</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -4598,13 +4742,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>170</v>
+        <v>65</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -4612,63 +4756,63 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>174</v>
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>182</v>
+        <v>69</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
@@ -4676,13 +4820,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>71</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
@@ -4690,13 +4834,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>184</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
@@ -4704,24 +4848,24 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>188</v>
+        <v>75</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
@@ -4729,24 +4873,24 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>192</v>
+        <v>77</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -4754,30 +4898,30 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>193</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>194</v>
+        <v>81</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -4785,13 +4929,13 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>195</v>
+        <v>83</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
@@ -4799,13 +4943,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>196</v>
+        <v>85</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -4813,13 +4957,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -4827,41 +4971,41 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>139</v>
+        <v>89</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>140</v>
+        <v>91</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
@@ -4869,13 +5013,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>141</v>
+        <v>93</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -4883,13 +5027,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>95</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -4897,13 +5041,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>143</v>
+        <v>97</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
@@ -4911,13 +5055,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>144</v>
+        <v>99</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
@@ -4925,35 +5069,35 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>145</v>
+        <v>101</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>
@@ -4962,7 +5106,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="n">
         <f aca="false">SUM(D2:D43)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished US41 and US42
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="212">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -204,12 +204,24 @@
     <t xml:space="preserve">Marriage after 14</t>
   </si>
   <si>
+    <t xml:space="preserve">US11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No bigamy</t>
+  </si>
+  <si>
     <t xml:space="preserve">US12</t>
   </si>
   <si>
     <t xml:space="preserve">Parents not too old</t>
   </si>
   <si>
+    <t xml:space="preserve">US13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sibling spacing</t>
+  </si>
+  <si>
     <t xml:space="preserve">US14</t>
   </si>
   <si>
@@ -294,348 +306,348 @@
     <t xml:space="preserve">List multiple births</t>
   </si>
   <si>
+    <t xml:space="preserve">US35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List recent births</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List recent deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List recent survivors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List upcoming birthdays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List upcoming anniversaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include partial dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reject illegitimate dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implemented in this sprint, and the minutes needed to write those lines of code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here's a sample burndown chart for a team of three:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remaining Stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Story Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Est Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Est Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep doing:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commit code regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrate code regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test regularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procrastination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad / dirty code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling in for people who need help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Being patient with less experienced programmers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discuss stories shortly in sprint meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assign similar stories to the same person although they might be difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarcasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having fun at our meetings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all multiple births in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all people in a GEDCOM file who were born in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage should not occur during marriage to another spouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siblings spacing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept and use dates without days or without days and months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Story Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WANT?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OWNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dates (birth, marriage, divorce, death) should not be after the current date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth should occur before marriage of an individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth should occur before death of an individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage should occur before death of either spouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divorce can only occur before death of both spouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child should be born before death of mother and before 9 months after death of father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No more than five siblings should be born at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There should be fewer than 15 siblings in a family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All male members of a family should have the same last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No marriages to descendants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents should not marry any of their descendants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siblings should not marry one another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First cousins should not marry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First cousins should not marry one another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aunts and uncles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aunts and uncles should not marry their nieces or nephews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Husband in family should be male and wife in family should be female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All individual IDs should be unique and all family IDs should be unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique families by spouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No more than one child with the same name and birth date should appear in a family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corresponding entries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include person's current age when listing individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List siblings in families by decreasing age, i.e. oldest siblings first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all deceased individuals in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living married people in a GEDCOM file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all living people over 30 who have never been married in a GEDCOM file</t>
+  </si>
+  <si>
     <t xml:space="preserve">US33</t>
   </si>
   <si>
     <t xml:space="preserve">List orphans</t>
   </si>
   <si>
-    <t xml:space="preserve">US35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List recent births</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List recent deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List recent survivors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List upcoming birthdays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List upcoming anniversaries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reject illegitimate dates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implemented in this sprint, and the minutes needed to write those lines of code.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Here's a sample burndown chart for a team of three:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remaining Stories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code Velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Act Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Act Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keep doing:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communicating regularly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commit code regularly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrate code regularly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test regularly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avoid:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procrastination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad / dirty code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filling in for people who need help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Being patient with less experienced programmers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discuss stories shortly in sprint meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assign similar stories to the same person although they might be difficult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarcasm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having fun at our meetings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all multiple births in a GEDCOM file</t>
-  </si>
-  <si>
     <t xml:space="preserve">List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
   </si>
   <si>
-    <t xml:space="preserve">List all people in a GEDCOM file who were born in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No bigamy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siblings spacing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WANT?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dates (birth, marriage, divorce, death) should not be after the current date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth should occur before marriage of an individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth should occur before death of an individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage should occur before death of either spouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divorce can only occur before death of both spouses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No more than five siblings should be born at the same time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There should be fewer than 15 siblings in a family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All male members of a family should have the same last name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No marriages to descendants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parents should not marry any of their descendants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siblings should not marry one another</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First cousins should not marry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First cousins should not marry one another</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aunts and uncles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aunts and uncles should not marry their nieces or nephews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Husband in family should be male and wife in family should be female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All individual IDs should be unique and all family IDs should be unique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique families by spouses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No more than one child with the same name and birth date should appear in a family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corresponding entries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include person's current age when listing individuals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List siblings in families by decreasing age, i.e. oldest siblings first</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all deceased individuals in a GEDCOM file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living married people in a GEDCOM file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all living people over 30 who have never been married in a GEDCOM file</t>
-  </si>
-  <si>
     <t xml:space="preserve">US34</t>
   </si>
   <si>
@@ -652,15 +664,6 @@
   </si>
   <si>
     <t xml:space="preserve">List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include partial dates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accept and use dates without days or without days and months</t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1032,11 +1035,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="81234050"/>
-        <c:axId val="41233526"/>
+        <c:axId val="52080701"/>
+        <c:axId val="51331454"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81234050"/>
+        <c:axId val="52080701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,14 +1071,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41233526"/>
+        <c:crossAx val="51331454"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41233526"/>
+        <c:axId val="51331454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,7 +1120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81234050"/>
+        <c:crossAx val="52080701"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1144,7 +1147,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1252,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="35786682"/>
-        <c:axId val="31576412"/>
+        <c:axId val="91312750"/>
+        <c:axId val="54931767"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35786682"/>
+        <c:axId val="91312750"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,14 +1288,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31576412"/>
+        <c:crossAx val="54931767"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31576412"/>
+        <c:axId val="54931767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35786682"/>
+        <c:crossAx val="91312750"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1372,9 +1375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>392040</xdr:colOff>
+      <xdr:colOff>391680</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1383,7 +1386,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4911480" cy="2662920"/>
+        <a:ext cx="4911120" cy="2662560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1402,9 +1405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>942480</xdr:colOff>
+      <xdr:colOff>942120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1414,7 +1417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1239120" cy="622080"/>
+          <a:ext cx="1238760" cy="621720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1506,9 +1509,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>492120</xdr:colOff>
+      <xdr:colOff>491760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1518,7 +1521,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1231560" cy="529200"/>
+          <a:ext cx="1231200" cy="528840"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1591,9 +1594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>56880</xdr:colOff>
+      <xdr:colOff>56520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1603,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1086840" cy="792720"/>
+          <a:ext cx="1086480" cy="792360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1676,9 +1679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>500760</xdr:colOff>
+      <xdr:colOff>500400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1688,7 +1691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="402840" cy="419040"/>
+          <a:ext cx="402480" cy="418680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1780,9 +1783,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>87120</xdr:colOff>
+      <xdr:colOff>86760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1792,7 +1795,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1073160" cy="736560"/>
+          <a:ext cx="1072800" cy="736200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1865,9 +1868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>619200</xdr:colOff>
+      <xdr:colOff>618840</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1877,7 +1880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1206360" cy="623520"/>
+          <a:ext cx="1206000" cy="623160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1955,9 +1958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>236160</xdr:colOff>
+      <xdr:colOff>235800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1966,7 +1969,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4804560" cy="2660040"/>
+        <a:ext cx="4804200" cy="2659680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1987,7 +1990,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2129,13 +2132,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.54"/>
@@ -2145,7 +2148,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2161,6 +2164,7 @@
       <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -2334,7 +2338,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>58</v>
@@ -2343,10 +2347,7 @@
         <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,7 +2369,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>62</v>
@@ -2377,10 +2378,7 @@
         <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2392,7 @@
         <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>39</v>
@@ -2411,7 +2409,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>39</v>
@@ -2428,7 +2426,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>39</v>
@@ -2436,7 +2434,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>70</v>
@@ -2445,7 +2443,7 @@
         <v>71</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>39</v>
@@ -2453,7 +2451,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>72</v>
@@ -2462,7 +2460,7 @@
         <v>73</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>39</v>
@@ -2496,7 +2494,7 @@
         <v>77</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>39</v>
@@ -2513,7 +2511,7 @@
         <v>79</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>39</v>
@@ -2530,7 +2528,7 @@
         <v>81</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>39</v>
@@ -2547,7 +2545,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>39</v>
@@ -2572,7 +2570,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>86</v>
@@ -2580,16 +2578,28 @@
       <c r="C26" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="D26" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>89</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,6 +2612,9 @@
       <c r="C28" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="D28" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -2613,6 +2626,9 @@
       <c r="C29" s="0" t="s">
         <v>93</v>
       </c>
+      <c r="D29" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -2624,6 +2640,9 @@
       <c r="C30" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="D30" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -2635,6 +2654,9 @@
       <c r="C31" s="0" t="s">
         <v>97</v>
       </c>
+      <c r="D31" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -2646,33 +2668,53 @@
       <c r="C32" s="0" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2708,32 +2750,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,27 +2783,27 @@
         <v>32</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>41065</v>
@@ -2777,7 +2819,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>41078</v>
@@ -2802,7 +2844,7 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>41092</v>
@@ -2827,7 +2869,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>41106</v>
@@ -2852,7 +2894,7 @@
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>41120</v>
@@ -2911,22 +2953,22 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,19 +3095,19 @@
         <v>36</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,7 +3136,7 @@
         <v>90</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,7 +3165,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3152,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,7 +3223,7 @@
         <v>90</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,7 +3252,7 @@
         <v>90</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,7 +3281,7 @@
         <v>70</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3268,7 +3310,7 @@
         <v>30</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,15 +3339,15 @@
         <v>180</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,12 +3362,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3333,27 +3375,27 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,12 +3403,12 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="11" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3414,19 +3456,19 @@
         <v>36</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,7 +3497,7 @@
         <v>240</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3484,15 +3526,15 @@
         <v>60</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>5</v>
@@ -3513,15 +3555,15 @@
         <v>180</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>5</v>
@@ -3542,15 +3584,15 @@
         <v>60</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>15</v>
@@ -3571,15 +3613,15 @@
         <v>60</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>15</v>
@@ -3600,15 +3642,15 @@
         <v>60</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>20</v>
@@ -3629,15 +3671,15 @@
         <v>80</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>20</v>
@@ -3658,16 +3700,16 @@
         <v>120</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,7 +3725,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,43 +3733,43 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,18 +3777,18 @@
     </row>
     <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="11" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3794,27 +3836,27 @@
         <v>36</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -3835,18 +3877,18 @@
         <v>60</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>39</v>
@@ -3864,15 +3906,15 @@
         <v>20</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
@@ -3893,15 +3935,15 @@
         <v>60</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>20</v>
@@ -3922,15 +3964,15 @@
         <v>10</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>20</v>
@@ -3951,15 +3993,15 @@
         <v>90</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
@@ -3980,18 +4022,18 @@
         <v>30</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>39</v>
@@ -4009,15 +4051,15 @@
         <v>30</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
@@ -4038,15 +4080,15 @@
         <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,7 +4103,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,47 +4111,47 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="11" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4117,17 +4159,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="11" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4146,10 +4188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4175,30 +4217,30 @@
         <v>36</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>20</v>
@@ -4212,19 +4254,19 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>60</v>
@@ -4232,19 +4274,19 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>60</v>
@@ -4252,56 +4294,56 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>60</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>25</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>25</v>
@@ -4312,19 +4354,19 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>60</v>
@@ -4332,16 +4374,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>30</v>
@@ -4352,13 +4394,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>25</v>
@@ -4372,25 +4414,24 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4409,8 +4450,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4435,19 +4476,19 @@
         <v>34</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -4459,7 +4500,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -4482,7 +4523,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -4505,7 +4546,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -4528,7 +4569,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -4551,7 +4592,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -4574,7 +4615,7 @@
         <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -4598,7 +4639,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -4621,7 +4662,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -4644,10 +4685,19 @@
         <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4658,21 +4708,30 @@
         <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>151</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -4683,21 +4742,30 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>180</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>155</v>
@@ -4714,72 +4782,105 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>180</v>
+        <v>20</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4806,10 +4907,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>187</v>
@@ -4817,13 +4918,22 @@
       <c r="D22" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>188</v>
@@ -4831,19 +4941,37 @@
       <c r="D23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>189</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4859,16 +4987,25 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4884,10 +5021,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>197</v>
@@ -4895,13 +5032,22 @@
       <c r="D28" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>198</v>
@@ -4910,15 +5056,21 @@
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>180</v>
+        <v>20</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>199</v>
@@ -4926,13 +5078,22 @@
       <c r="D30" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>200</v>
@@ -4940,167 +5101,206 @@
       <c r="D31" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E31" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E33" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>88</v>
+        <v>203</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>89</v>
+        <v>204</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E36" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E37" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E38" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E39" s="0" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E40" s="0" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>208</v>
+        <v>103</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>209</v>
+        <v>104</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>210</v>
+        <v>157</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add execution for us 32
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -930,7 +930,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1035,11 +1035,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="63560150"/>
-        <c:axId val="23147924"/>
+        <c:axId val="38770992"/>
+        <c:axId val="76927751"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63560150"/>
+        <c:axId val="38770992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,14 +1071,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23147924"/>
+        <c:crossAx val="76927751"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23147924"/>
+        <c:axId val="76927751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63560150"/>
+        <c:crossAx val="38770992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1147,7 +1147,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1252,11 +1252,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="62888069"/>
-        <c:axId val="83138354"/>
+        <c:axId val="9395742"/>
+        <c:axId val="37804416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62888069"/>
+        <c:axId val="9395742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1288,14 +1288,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83138354"/>
+        <c:crossAx val="37804416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83138354"/>
+        <c:axId val="37804416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62888069"/>
+        <c:crossAx val="9395742"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1375,9 +1375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>391320</xdr:colOff>
+      <xdr:colOff>390960</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1386,7 +1386,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4910760" cy="2662200"/>
+        <a:ext cx="4910400" cy="2661840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1405,9 +1405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>941760</xdr:colOff>
+      <xdr:colOff>941400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1417,7 +1417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1238400" cy="621360"/>
+          <a:ext cx="1238040" cy="621000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1509,9 +1509,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>491400</xdr:colOff>
+      <xdr:colOff>491040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,7 +1521,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1230840" cy="528480"/>
+          <a:ext cx="1230480" cy="528120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1594,9 +1594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>56160</xdr:colOff>
+      <xdr:colOff>55800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1606,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1086120" cy="792000"/>
+          <a:ext cx="1085760" cy="791640"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1679,9 +1679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>500040</xdr:colOff>
+      <xdr:colOff>499680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1691,7 +1691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="402120" cy="418320"/>
+          <a:ext cx="401760" cy="417960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1783,9 +1783,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1795,7 +1795,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1072440" cy="735840"/>
+          <a:ext cx="1072080" cy="735480"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1868,9 +1868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>618480</xdr:colOff>
+      <xdr:colOff>618120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1880,7 +1880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1205640" cy="622800"/>
+          <a:ext cx="1205280" cy="622440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1958,9 +1958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1969,7 +1969,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4803840" cy="2659320"/>
+        <a:ext cx="4803480" cy="2658960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4191,7 +4191,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4249,6 +4249,12 @@
         <v>15</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished filling a couple things out
</commit_message>
<xml_diff>
--- a/Team08Report.xlsx
+++ b/Team08Report.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="212">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -1035,11 +1035,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="25468906"/>
-        <c:axId val="98313504"/>
+        <c:axId val="93628413"/>
+        <c:axId val="24057431"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25468906"/>
+        <c:axId val="93628413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,14 +1071,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98313504"/>
+        <c:crossAx val="24057431"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98313504"/>
+        <c:axId val="24057431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25468906"/>
+        <c:crossAx val="93628413"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1252,11 +1252,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="32686353"/>
-        <c:axId val="84669033"/>
+        <c:axId val="10880224"/>
+        <c:axId val="60349169"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32686353"/>
+        <c:axId val="10880224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1288,14 +1288,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84669033"/>
+        <c:crossAx val="60349169"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84669033"/>
+        <c:axId val="60349169"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32686353"/>
+        <c:crossAx val="10880224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1375,9 +1375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>390600</xdr:colOff>
+      <xdr:colOff>390240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1386,7 +1386,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3629160"/>
-        <a:ext cx="4910040" cy="2661480"/>
+        <a:ext cx="4909680" cy="2661120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1405,9 +1405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>941040</xdr:colOff>
+      <xdr:colOff>940680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1417,7 +1417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1512720"/>
-          <a:ext cx="1237680" cy="620640"/>
+          <a:ext cx="1237320" cy="620280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1509,9 +1509,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>490680</xdr:colOff>
+      <xdr:colOff>490320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,7 +1521,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5582520" y="1487160"/>
-          <a:ext cx="1230120" cy="527760"/>
+          <a:ext cx="1229760" cy="527400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1594,9 +1594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>55440</xdr:colOff>
+      <xdr:colOff>55080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1606,7 +1606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2879640" y="1316520"/>
-          <a:ext cx="1085400" cy="791280"/>
+          <a:ext cx="1085040" cy="790920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1679,9 +1679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>499320</xdr:colOff>
+      <xdr:colOff>498960</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1691,7 +1691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1639440"/>
-          <a:ext cx="401400" cy="417600"/>
+          <a:ext cx="401040" cy="417240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1783,9 +1783,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>85320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1795,7 +1795,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4481640" y="1338840"/>
-          <a:ext cx="1071720" cy="735120"/>
+          <a:ext cx="1071360" cy="734760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1868,9 +1868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>617760</xdr:colOff>
+      <xdr:colOff>617400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1880,7 +1880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5734800" y="5127840"/>
-          <a:ext cx="1204920" cy="622080"/>
+          <a:ext cx="1204560" cy="621720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1958,9 +1958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>234720</xdr:colOff>
+      <xdr:colOff>234360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1969,7 +1969,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1470600"/>
-        <a:ext cx="4803120" cy="2658600"/>
+        <a:ext cx="4802760" cy="2658240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4190,8 +4190,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4245,6 +4245,9 @@
       <c r="D2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F2" s="0" t="n">
         <v>15</v>
       </c>
@@ -4256,6 +4259,9 @@
       </c>
       <c r="I2" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4311,6 +4317,9 @@
       <c r="D5" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="0" t="n">
         <v>25</v>
       </c>
@@ -4322,6 +4331,9 @@
       </c>
       <c r="I5" s="0" t="n">
         <v>135</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4377,6 +4389,9 @@
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="0" t="n">
         <v>30</v>
       </c>
@@ -4388,6 +4403,9 @@
       </c>
       <c r="I8" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4443,6 +4461,9 @@
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F11" s="0" t="n">
         <v>15</v>
       </c>
@@ -4454,6 +4475,9 @@
       </c>
       <c r="I11" s="0" t="n">
         <v>120</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>